<commit_message>
se actualiza carpeta de reporte
</commit_message>
<xml_diff>
--- a/tareas/zippas_omp/report/perf_report.xlsx
+++ b/tareas/zippas_omp/report/perf_report.xlsx
@@ -546,8 +546,8 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="60042193"/>
-        <c:axId val="72882414"/>
+        <c:axId val="9689"/>
+        <c:axId val="81038360"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -709,50 +709,16 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="17870048"/>
-        <c:axId val="54920884"/>
+        <c:axId val="75332692"/>
+        <c:axId val="87180371"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="60042193"/>
+        <c:axId val="9689"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Título del eje</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -779,7 +745,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72882414"/>
+        <c:crossAx val="81038360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -787,7 +753,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72882414"/>
+        <c:axId val="81038360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="900"/>
@@ -861,12 +827,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60042193"/>
+        <c:crossAx val="9689"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="17870048"/>
+        <c:axId val="75332692"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -898,14 +864,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54920884"/>
+        <c:crossAx val="87180371"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="54920884"/>
+        <c:axId val="87180371"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -968,7 +934,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17870048"/>
+        <c:crossAx val="75332692"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1185,8 +1151,8 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="1278209"/>
-        <c:axId val="74608698"/>
+        <c:axId val="74538311"/>
+        <c:axId val="56092907"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1312,50 +1278,16 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="94524885"/>
-        <c:axId val="36349065"/>
+        <c:axId val="6000079"/>
+        <c:axId val="5066932"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1278209"/>
+        <c:axId val="74538311"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>Título del eje</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1382,7 +1314,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74608698"/>
+        <c:crossAx val="56092907"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1390,7 +1322,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74608698"/>
+        <c:axId val="56092907"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1463,12 +1395,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1278209"/>
+        <c:crossAx val="74538311"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="94524885"/>
+        <c:axId val="6000079"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1500,14 +1432,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36349065"/>
+        <c:crossAx val="5066932"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="36349065"/>
+        <c:axId val="5066932"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1570,7 +1502,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94524885"/>
+        <c:crossAx val="6000079"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1793,8 +1725,8 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="86284891"/>
-        <c:axId val="17010725"/>
+        <c:axId val="64872842"/>
+        <c:axId val="2944840"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1926,11 +1858,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="32574507"/>
-        <c:axId val="36836522"/>
+        <c:axId val="12061019"/>
+        <c:axId val="3449212"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="86284891"/>
+        <c:axId val="64872842"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1957,7 +1889,7 @@
                     </a:solidFill>
                     <a:latin typeface="Calibri"/>
                   </a:rPr>
-                  <a:t>Título del eje</a:t>
+                  <a:t>Cantidad de Hilos</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1996,7 +1928,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17010725"/>
+        <c:crossAx val="2944840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2004,7 +1936,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="17010725"/>
+        <c:axId val="2944840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2077,12 +2009,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86284891"/>
+        <c:crossAx val="64872842"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="32574507"/>
+        <c:axId val="12061019"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2114,14 +2046,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36836522"/>
+        <c:crossAx val="3449212"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="36836522"/>
+        <c:axId val="3449212"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2184,7 +2116,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32574507"/>
+        <c:crossAx val="12061019"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2407,8 +2339,8 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="79823142"/>
-        <c:axId val="36897397"/>
+        <c:axId val="97406183"/>
+        <c:axId val="82901422"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2540,11 +2472,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="84822277"/>
-        <c:axId val="98665670"/>
+        <c:axId val="65867874"/>
+        <c:axId val="96468037"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="79823142"/>
+        <c:axId val="97406183"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2571,7 +2503,7 @@
                     </a:solidFill>
                     <a:latin typeface="Calibri"/>
                   </a:rPr>
-                  <a:t>Título del eje</a:t>
+                  <a:t>Cantidad de Hilos</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2610,7 +2542,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36897397"/>
+        <c:crossAx val="82901422"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2618,7 +2550,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="36897397"/>
+        <c:axId val="82901422"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2691,12 +2623,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79823142"/>
+        <c:crossAx val="97406183"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="84822277"/>
+        <c:axId val="65867874"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2728,14 +2660,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98665670"/>
+        <c:crossAx val="96468037"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98665670"/>
+        <c:axId val="96468037"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2798,7 +2730,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84822277"/>
+        <c:crossAx val="65867874"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2861,9 +2793,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>304200</xdr:colOff>
+      <xdr:colOff>303840</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>104040</xdr:rowOff>
+      <xdr:rowOff>103680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2873,7 +2805,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4686480" y="961920"/>
-          <a:ext cx="304200" cy="304200"/>
+          <a:ext cx="303840" cy="303840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2901,9 +2833,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>304200</xdr:colOff>
+      <xdr:colOff>303840</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>104040</xdr:rowOff>
+      <xdr:rowOff>103680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2913,7 +2845,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="937440" y="762120"/>
-          <a:ext cx="304200" cy="303840"/>
+          <a:ext cx="303840" cy="303480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2941,9 +2873,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>936000</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>189720</xdr:rowOff>
+      <xdr:colOff>935640</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>190440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2952,7 +2884,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="1874520" y="2554920"/>
-        <a:ext cx="6559560" cy="2864160"/>
+        <a:ext cx="6559200" cy="3055320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2971,9 +2903,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>923040</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:colOff>922680</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>190440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2982,7 +2914,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="1879200" y="6401160"/>
-        <a:ext cx="6541920" cy="3020400"/>
+        <a:ext cx="6541560" cy="3228480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3001,9 +2933,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>16920</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>189720</xdr:rowOff>
+      <xdr:colOff>16560</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>13680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3012,7 +2944,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="8436600" y="2552760"/>
-        <a:ext cx="5639400" cy="2866320"/>
+        <a:ext cx="5639040" cy="3071160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3031,9 +2963,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>14400</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>2880</xdr:rowOff>
+      <xdr:colOff>14040</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>13680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3042,7 +2974,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="14079240" y="2553840"/>
-        <a:ext cx="5617800" cy="2868840"/>
+        <a:ext cx="5617440" cy="3070080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3062,8 +2994,8 @@
   </sheetPr>
   <dimension ref="B5:U33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L35" activeCellId="0" sqref="L35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R33" activeCellId="0" sqref="R33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>